<commit_message>
Se agrega contraseña a los perfiles de implementacion, se finaliza 9989
</commit_message>
<xml_diff>
--- a/src/Sofco.WebApi/wwwroot/excelTemplates/worktime-control-hours.xlsx
+++ b/src/Sofco.WebApi/wwwroot/excelTemplates/worktime-control-hours.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\GAPS\src\Sofco.WebApi\wwwroot\excelTemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GAPS\Fuentes\GAPS\src\Sofco.WebApi\wwwroot\excelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12468"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12465"/>
   </bookViews>
   <sheets>
     <sheet name="Analiticas-Recurso" sheetId="1" r:id="rId1"/>
@@ -153,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -161,10 +161,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,65 +450,61 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.19921875" customWidth="1"/>
+    <col min="1" max="1" width="27.25" customWidth="1"/>
     <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="4" max="4" width="15.19921875" customWidth="1"/>
-    <col min="5" max="5" width="14.59765625" customWidth="1"/>
-    <col min="6" max="6" width="18.69921875" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="13.69921875" customWidth="1"/>
-    <col min="9" max="9" width="15.69921875" customWidth="1"/>
-    <col min="10" max="10" width="10.09765625" customWidth="1"/>
+    <col min="4" max="4" width="15.25" style="10" customWidth="1"/>
+    <col min="5" max="5" width="14.625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="18.75" style="10" customWidth="1"/>
+    <col min="7" max="7" width="15" style="10" customWidth="1"/>
+    <col min="8" max="8" width="13.75" style="10" customWidth="1"/>
+    <col min="9" max="9" width="15.75" customWidth="1"/>
+    <col min="10" max="10" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="8"/>
       <c r="C1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
       <c r="I1" s="5"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="9"/>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="9"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="10"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="10"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D3" s="9"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,26 +514,26 @@
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="12" t="s">
         <v>20</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" s="2"/>
     </row>
   </sheetData>
@@ -551,18 +549,18 @@
       <selection activeCell="G2" sqref="A2:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.69921875" customWidth="1"/>
-    <col min="2" max="2" width="14.09765625" customWidth="1"/>
-    <col min="3" max="3" width="26.59765625" customWidth="1"/>
+    <col min="1" max="1" width="45.75" customWidth="1"/>
+    <col min="2" max="2" width="14.125" customWidth="1"/>
+    <col min="3" max="3" width="26.625" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
-    <col min="5" max="5" width="29.09765625" customWidth="1"/>
-    <col min="6" max="6" width="29.69921875" customWidth="1"/>
-    <col min="7" max="7" width="7.69921875" customWidth="1"/>
+    <col min="5" max="5" width="29.125" customWidth="1"/>
+    <col min="6" max="6" width="29.75" customWidth="1"/>
+    <col min="7" max="7" width="7.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -585,7 +583,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>

</xml_diff>